<commit_message>
making a modular version of my maximum liklihood estimation script
</commit_message>
<xml_diff>
--- a/Climbing_Stats_ProjectVersion.xlsx
+++ b/Climbing_Stats_ProjectVersion.xlsx
@@ -1841,7 +1841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -3197,6 +3197,56 @@
         <v>6</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" t="n">
+        <v>9</v>
+      </c>
+      <c r="C27" t="n">
+        <v>32</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>